<commit_message>
Update test bug testPlan
</commit_message>
<xml_diff>
--- a/Tests_Documentation/TestCases_1.1.xlsx
+++ b/Tests_Documentation/TestCases_1.1.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\chris\source\repos\Portfolio\Python\MODFLOW\MODFLOW\Tests_Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36D4857D-EDE0-47E5-B66A-5FA95D46C400}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9B6FD4C4-EA33-4BE5-8A0E-36A3F30F725A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="20370" yWindow="-2595" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -147,9 +147,6 @@
     <t>3.2</t>
   </si>
   <si>
-    <t xml:space="preserve">Validate whether user is possible to import a project           </t>
-  </si>
-  <si>
     <t>4.1</t>
   </si>
   <si>
@@ -159,9 +156,6 @@
     <t>4.2</t>
   </si>
   <si>
-    <t>Click on File-&gt;Import Project</t>
-  </si>
-  <si>
     <t>4.3</t>
   </si>
   <si>
@@ -181,6 +175,12 @@
   </si>
   <si>
     <t>Desktop Notes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Validate whether user is possible to open an existing project           </t>
+  </si>
+  <si>
+    <t>Click on File-&gt;Open Project</t>
   </si>
 </sst>
 </file>
@@ -620,7 +620,7 @@
   <dimension ref="A1:H142"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="12.75"/>
@@ -645,10 +645,10 @@
         <v>2</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>3</v>
@@ -941,7 +941,7 @@
         <v>4</v>
       </c>
       <c r="B17" s="15" t="s">
-        <v>38</v>
+        <v>48</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="15"/>
@@ -952,10 +952,10 @@
     </row>
     <row r="18" spans="1:8">
       <c r="A18" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="B18" s="16" t="s">
         <v>39</v>
-      </c>
-      <c r="B18" s="16" t="s">
-        <v>40</v>
       </c>
       <c r="C18" s="16"/>
       <c r="D18" s="12" t="s">
@@ -970,10 +970,10 @@
     </row>
     <row r="19" spans="1:8">
       <c r="A19" s="9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B19" s="11" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C19" s="11"/>
       <c r="D19" s="12" t="s">
@@ -988,10 +988,10 @@
     </row>
     <row r="20" spans="1:8">
       <c r="A20" s="9" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B20" s="11" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C20" s="11"/>
       <c r="D20" s="12" t="s">
@@ -1004,13 +1004,13 @@
     </row>
     <row r="21" spans="1:8">
       <c r="A21" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="C21" s="11" t="s">
         <v>45</v>
-      </c>
-      <c r="B21" s="11" t="s">
-        <v>46</v>
-      </c>
-      <c r="C21" s="11" t="s">
-        <v>47</v>
       </c>
       <c r="D21" s="12" t="s">
         <v>9</v>

</xml_diff>